<commit_message>
cap nhat bo sung tinh luong
</commit_message>
<xml_diff>
--- a/Data/102018/nangsuat.xlsx
+++ b/Data/102018/nangsuat.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DucTn\Desktop\luong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF003276-EC5F-49EA-B67A-D456BE5F6112}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CB9161-0ED1-4E8C-9D46-8C87F86BB8CC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -423,10 +424,10 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L32" sqref="L32"/>
+      <selection pane="bottomRight" activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -491,11 +492,10 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="4">
-        <v>9124</v>
+        <v>8524</v>
       </c>
       <c r="K2">
-        <f>180+420+400</f>
-        <v>1000</v>
+        <v>1600</v>
       </c>
       <c r="L2" s="3"/>
     </row>
@@ -609,8 +609,7 @@
         <v>25120</v>
       </c>
       <c r="G6" s="3">
-        <f>9840+6020</f>
-        <v>15860</v>
+        <v>8275</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="3"/>
@@ -668,7 +667,9 @@
         <v>30210</v>
       </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="4"/>
+      <c r="H8" s="4">
+        <v>1030</v>
+      </c>
       <c r="I8" s="3"/>
       <c r="J8" s="4">
         <v>25000</v>
@@ -715,12 +716,9 @@
         <v>21310</v>
       </c>
       <c r="C10" s="3">
-        <f>2470+460+3645</f>
-        <v>6575</v>
-      </c>
-      <c r="D10" s="3">
-        <v>470</v>
-      </c>
+        <v>5108</v>
+      </c>
+      <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3">
         <v>23060</v>
@@ -850,7 +848,7 @@
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="4">
-        <v>52200</v>
+        <v>20250</v>
       </c>
       <c r="K14" s="4">
         <f>1250+30700</f>
@@ -866,9 +864,11 @@
         <v>43387</v>
       </c>
       <c r="B15" s="3">
-        <v>23460</v>
-      </c>
-      <c r="C15" s="3"/>
+        <v>21800</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1660</v>
+      </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3">
@@ -937,11 +937,10 @@
       <c r="H17" s="4"/>
       <c r="I17" s="3"/>
       <c r="J17" s="4">
-        <v>10680</v>
+        <v>8490</v>
       </c>
       <c r="K17" s="4">
-        <f>320+6540</f>
-        <v>6860</v>
+        <v>10050</v>
       </c>
       <c r="L17" s="3"/>
     </row>
@@ -974,7 +973,7 @@
         <v>1710</v>
       </c>
       <c r="L18" s="3">
-        <v>300</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1158,16 +1157,13 @@
         <v>18550</v>
       </c>
       <c r="G25" s="3"/>
-      <c r="H25" s="4">
-        <f>2700</f>
-        <v>2700</v>
-      </c>
+      <c r="H25" s="4"/>
       <c r="I25" s="3"/>
       <c r="J25" s="4">
-        <v>14060</v>
+        <v>6060</v>
       </c>
       <c r="K25" s="4">
-        <v>8590</v>
+        <v>16590</v>
       </c>
       <c r="L25" s="3"/>
     </row>
@@ -1234,8 +1230,7 @@
         <v>15650</v>
       </c>
       <c r="C28" s="3">
-        <f>1700+800</f>
-        <v>2500</v>
+        <v>9700</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -1387,4 +1382,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE12458-54E4-472A-B1AE-096A6AF5E780}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>